<commit_message>
Mise en ligne officielle
Correction de bugs, amélioration de l'ergonomie et ajout de pages d'information
</commit_message>
<xml_diff>
--- a/data/meta.xlsx
+++ b/data/meta.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="675" windowWidth="20730" windowHeight="11520" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="735" windowWidth="20730" windowHeight="11460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Selection2019!$B$1:$K$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Selection2019!$B$1:$L$14</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="133">
   <si>
     <t>Champ</t>
   </si>
@@ -211,15 +211,6 @@
     <t>Formation</t>
   </si>
   <si>
-    <t>DEPP 2015</t>
-  </si>
-  <si>
-    <t>RP 2015 (Insee)</t>
-  </si>
-  <si>
-    <t>Insee-RP 2015, METRIC 2016</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -265,9 +256,6 @@
     <t>calculé</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Indicateur_s</t>
   </si>
   <si>
@@ -310,33 +298,6 @@
     <t>pour 100 enfants</t>
   </si>
   <si>
-    <t>Part des élèves de niveau 1ère
-inscrits dans des formations
-non mixtes</t>
-  </si>
-  <si>
-    <t>Part des emplois dans des
-catégories socioprofessionnelles
-non-mixtes</t>
-  </si>
-  <si>
-    <t>Part des femmes peu ou pas
-diplômées</t>
-  </si>
-  <si>
-    <t>Taux de couverture global 
-accueil jeune enfant</t>
-  </si>
-  <si>
-    <t>Part des 6-10 ans scolarisés
-hors de leur commune
-de résidence</t>
-  </si>
-  <si>
-    <t>Part des ménages avec 3 enfants
-ou plus</t>
-  </si>
-  <si>
     <t>Familles nombreuses</t>
   </si>
   <si>
@@ -352,54 +313,184 @@
     <t>Taux de chômage</t>
   </si>
   <si>
-    <t>Part des emplois
-à temps partiel</t>
-  </si>
-  <si>
-    <t>Part des emplois
-en contrat précaire</t>
-  </si>
-  <si>
-    <t>Temps moyen de trajet
-domicile-travail des femmes</t>
-  </si>
-  <si>
     <t>Trajet domicile-travail des femmes</t>
   </si>
   <si>
-    <t>EQU_4</t>
-  </si>
-  <si>
-    <t>Accès aux équipements</t>
-  </si>
-  <si>
-    <t>Insee-BPE 2017, Insee-RP 2015, Insee-METRIC 2017</t>
-  </si>
-  <si>
     <t>Éloignement de l'école</t>
   </si>
   <si>
-    <t>Part des 15-24 ans
-ni en emploi,
-ni en études</t>
-  </si>
-  <si>
-    <t>Part des familles monoparentales
-parmi l'ensemble des familles</t>
-  </si>
-  <si>
     <t>Inactivité</t>
   </si>
   <si>
-    <t>Part des inactifs parmi les 15-64 ans
-(hors étudiants et retraités)</t>
-  </si>
-  <si>
-    <t>Part de la population
-ayant accès en moyenne
-aux 12 équipements
-de la gamme intermédiaire
-en plus de 15 minutes</t>
+    <t>CAF 2015, Insee-RP 2015</t>
+  </si>
+  <si>
+    <t>EPCI 2018</t>
+  </si>
+  <si>
+    <t>Typologie de l'accès à l'emploi des femmes et de ses principaux freins</t>
+  </si>
+  <si>
+    <t>TYPO</t>
+  </si>
+  <si>
+    <t>Typologie</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Insee-RP 2015, CAF 2015</t>
+  </si>
+  <si>
+    <t>Insee-RP 2015</t>
+  </si>
+  <si>
+    <t>DEPP-Base scolarité 2015</t>
+  </si>
+  <si>
+    <t>Insee-RP 2015, Insee-METRIC 2016</t>
+  </si>
+  <si>
+    <t>aucune</t>
+  </si>
+  <si>
+    <t>Part des inactifs parmi les 15-64 ans (hors étudiants et retraités)</t>
+  </si>
+  <si>
+    <t>Part des emplois à temps partiel</t>
+  </si>
+  <si>
+    <t>Part des emplois en contrat précaire</t>
+  </si>
+  <si>
+    <t>Part des familles monoparentales parmi l'ensemble des familles</t>
+  </si>
+  <si>
+    <t>Part des ménages avec 3 enfants ou plus</t>
+  </si>
+  <si>
+    <t>Part des emplois dans des catégories socioprofessionnelles non-mixtes</t>
+  </si>
+  <si>
+    <t>Part des élèves de niveau 1ère inscrits dans des formations non mixtes</t>
+  </si>
+  <si>
+    <t>Part des femmes peu ou pas diplômées</t>
+  </si>
+  <si>
+    <t>Part des enfants de moins de 3 ans n'ayant théoriquement pas de place d'accueil</t>
+  </si>
+  <si>
+    <t>Part des 6-10 ans scolarisés hors de leur commune de résidence</t>
+  </si>
+  <si>
+    <t>Temps moyen de trajet domicile-travail des femmes</t>
+  </si>
+  <si>
+    <t>Part des 15-24 ans ni en emploi, ni en études, ni en formation</t>
+  </si>
+  <si>
+    <t>Le taux de chômage correspond au nombre total de chômeurs rapporté au nombre total d'actifs. Il s'agit d'un indicateur d'accès à l'emploi qui dispose d'une déclinaison sexuée. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;14,7 % pour les femmes&lt;/strong&gt; contre &lt;strong&gt;13,5% pour les hommes&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+&lt;i&gt;Attention :  le taux de chômage utilisé ici est celui du recensement de l'Insee ; il s'agit donc d'un taux de chômage "déclaratif", ce qui explique les écarts avec le taux de chômage au sens du BIT. Ce choix est justifié par le fait que le taux de chômage au sens du recensement est le seul qui permette d'avoir une analyse au niveau des EPCI.&lt;/i&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Cet indicateur est obtenu en rapportant le nombre d'inactifs de 15 à 64 ans (hors retraités et étudiants) au nombre total de personnes âgées de 15 à 64 ans. Il s'agit d'un indicateur d'accès à l'emploi qui dispose d'une déclinaison sexuée. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;11,6 % pour les femmes&lt;/strong&gt; contre &lt;strong&gt;5,5% pour les hommes&lt;/strong&gt; soit &lt;strong&gt;2,1 fois plus&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+La part d'inactifs (hors retraités et étudiants) permet d'apprécier la proportion de personnes qui se situent en-dehors du marché du travail  de façon durable (par choix ou non).&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>La part des emplois à temps partiel correspond au nombre d'emplois au lieu de travail occupés à temps partiel sur le nombre total d'emplois au lieu de travail. Il s'agit d'un indicateur d'accès à l'emploi qui dispose d'une déclinaison sexuée. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;27,4 % pour les femmes&lt;/strong&gt; contre &lt;strong&gt;8,2% pour les hommes&lt;/strong&gt; soit &lt;strong&gt;3,3 fois plus&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+Il s'agit d'un indicateur de conditions d'emploi. Le temps partiel peut être subi ou choisi. Il peut également correspondre à des temps de travail différents : 50%, 80%,...Dans tous les cas, il se traduit par une rémunération moindre par rapport aux emplois à temps complet.&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>La part des emplois en contrat précaire correspond au nombre d'emplois salariés au lieu de travail faisant l'objet d'un contrat autre qu'un CDI (CDD, contrat d'apprentissage, contrat d'interim, stages rémunérés,...), rapporté au nombre total d'emplois salariés au lieu de travail. Il s'agit d'un indicateur d'accès à l'emploi qui dispose d'une déclinaison sexuée. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;16,0 % pour les femmes&lt;/strong&gt; contre &lt;strong&gt;14,5% pour les hommes&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>La part des 15-24 ans ni en emploi, ni en études, ni en formation correspond à l'ensemble des jeunes de 15 à 24 ans sortis du système scolaire mais qui n'ont pas d'emploi. Il s'agit d'un indicateur d'accès à l'emploi qui dispose d'une déclinaison sexuée. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;16,9 % pour les femmes&lt;/strong&gt; contre &lt;strong&gt;17,9% pour les hommes&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+Cet indicateur permet de mesurer le degré d'insertion des jeunes sur un territoire donné. Dans le contexte européen, on utilise souvent l'expression de "NEET" (Not in Education, Employment or Training) pour qualifier ces jeunes inactifs.&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>La part des familles monoparentales rend compte du nombre de familles monoparentales rapporté au nombre total de familles. Il s'agit d'un indicateur de frein potentiel à l'accès à l'emploi des femmes. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;15,6%&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+Les familles monoparentales sont à 85% composées d'une mère et de ses enfants. Les parents seuls et en particulier les mères seules rencontrent plus souvent des difficultés d'insertion professionnelle et sont plus souvent inactifs, au chômage ou précaires. La difficulté rencontrée par les parents isolés à trouver un emploi stable s'explique par la complexité à combiner vie familiale et vie professionnelle, d'autant plus que les familles monoparentales ont plus souvent des difficultés financières et appartiennent plus souvent à des catégories socio-professionnelles moins favorisées.&lt;br/&gt;&lt;br/&gt;
+Pour aller plus loin : &lt;a href = 'https://drees.solidarites-sante.gouv.fr/etudes-et-statistiques/publications/les-dossiers-de-la-drees/dossiers-solidarite-et-sante/article/les-familles-monoparentales-depuis-1990' target = '_blank'&gt;Marie ACS, Bertrand LHOMMEAU, Émilie RAYNAUD. 2015, « Les familles monoparentales depuis 1990 », Dossiers Solidarité Santé n°67, Drees, Juillet.&lt;/a&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>La part des familles nombreuses est obtenue en rapportant le nombre de familles composées de 3 enfants ou plus au nombre total de familles. Il s'agit d'un indicateur de frein potentiel à l'accès à l'emploi des femmes. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;9,4%&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+Les mères de familles nombreuses, plus souvent touchées par la pauvreté et faiblement diplômées, sont davantage inactives et concernées par le temps partiel.&lt;br/&gt;&lt;br/&gt;
+Pour aller plus loin : &lt;a href = 'https://www.insee.fr/fr/statistiques/1283771' target = '_blank'&gt;Nathalie BLANPAIN, Liliane LINCOT. 2015, « Avoir trois enfants ou plus à la maison », Insee Première n°1531, Insee, Janvier.&lt;/a&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'indicateur de non mixité de l'offre d'emploi correspond à la part d'emplois occupés au lieu de travail dans une catégorie socio-professionnelle (CSP en 29 postes) non mixte localement. On définit ici comme non mixte une catégorie socio-professionnelle pour laquelle le taux de féminisation (la part des emplois occupés par des femmes sur le total d'emplois occupés) est soit inférieur à 33%, soit supérieur à 63%. Ces bornes correspondent à un écart de plus ou moins 15 points de part et d'autre du taux de féminisation total de l'emploi qui est de 48%. Les taux de féminisation sont mesurés localement pour chaque EPCI. Ainsi, une CSP peut être mixte à l'échelle nationale mais non mixte à l'échelle d'une intercommunalité et inversement.  Il s'agit d'un indicateur de frein potentiel à l'accès à l'emploi des femmes. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;73,7%&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+En France, près de 3 emplois occupés sur 4 le sont dans des catégories socio-professionnelles non mixtes, c'est-à-dire où le taux de féminisation est soit particulièrement bas (comme les chauffeurs avec un taux de féminisation de 8,7% ), soit particulièrement élevé (comme  les personnels des services aux particuliers avec un taux de féminisation de 85,7%). Localement, la non mixité du tissu de l'emploi peut être un obstacle à l'emploi des femmes qui ont alors de moindres posssibilités d'embauche. La non mixité de l'emploi concerne les hommes de la même façon.&lt;br/&gt;&lt;br/&gt;
+&lt;i&gt;Attention : il convient de préciser que le recours aux catégories socio-professionnelles se justifie par les besoins de l'analyse territorialisée. Couramment, la mixité de l'emploi est plutôt appréhendée à partir des "métiers" déclinés en 87 postes.&lt;/i&gt;&lt;br/&gt;&lt;br/&gt;
+Pour aller plus loin : &lt;a href = 'https://dares.travail-emploi.gouv.fr/dares-etudes-et-statistiques/etudes-et-syntheses/dares-analyses-dares-indicateurs-dares-resultats/article/la-repartition-des-hommes-et-des-femmes-par-metiers' target = '_blank'&gt;Julie ARGOUARC'H, Oana CALAVREZO. 2013, « La répartition des hommes et des femmes par métiers. Une baisse de la ségrégation depuis 30 ans », Dares Analyses n°79, Dares, Décembre.&lt;/a&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;
+</t>
+  </si>
+  <si>
+    <t>L'indicateur de non mixité de l'offre de formation de niveau 1ère correspond à la proportion d'élèves de niveau 1ère (toutes filières confondues) inscrits dans des formations non mixtes. Les filières considérés comme "non mixtes" sont les filières où le taux de féminisation est soit inférieur à 35%, soit supérieur à 65%. Ces bornes correspondent à un écart de plus ou moins 15 points de part et d'autre du taux de féminisation global des élèves de niveau 1ère (50%).  Les taux de féminisation sont mesurés localement pour chaque EPCI. Ainsi, une formation peut être mixte à l'échelle nationale mais non mixte à l'échelle d'une intercommunalité et inversement.  Il s'agit d'un indicateur de frein potentiel à l'accès à l'emploi des femmes. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;47,6%&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+En France, près d'1 élève de première sur 2 est inscrit dans une formation qui peut être considérée comme non mixte, soit parce que le taux de féminisation y est particulièrement bas (comme les 1ères professionnelles des domaines de la production avec un taux de féminisation de 11,6%) soit particulièrement haut (comme les 1ères ST2S-SMS des domaines des services ou les premières L avec des taux de féminisation de respectivement 88,4% et 79,6%). A l'entrée dans la vie professionnelle, le caractère mixte ou non des formations suivies se traduit directement dans la plus ou moins grande mixité des métiers. Les élèves de première qui suivent une formation professionnalisante sont particulièrement concernés par le phénomène et c'est dans les catégories socio-professionnelles auxquels ils sont majoritairement destinés - les ouvriers et les employés - que l'on retrouve les taux de féminisation les plus éloignés de la moyenne.&lt;br/&gt;&lt;br/&gt;
+&lt;i&gt;Attention : 44% des intercommunalités ne disposent d'aucun établissement accueillant des formations de niveau 1ère. Pour ces intercommunalités, on a affecté la valeur de l'EPCI où sont scolarisés la majorité des élèves de niveau 1ère résidant dans l'EPCI.&lt;/i&gt;&lt;br/&gt;&lt;br/&gt;
+Pour aller plus loin : &lt;a href = 'https://www.education.gouv.fr/cid57113/filles-et-garcons-sur-le-chemin-de-l-egalite-de-l-ecole-a-l-enseignement-superieur-edition-2018.html' target = '_blank'&gt;DEPP, Filles et garçons sur le chemin de l'égalité de l'école à l'enseignement supérieur 2019&lt;/a&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>La part des femmes peu ou pas diplômées correspond à l'ensemble des femmes non scolarisées de 15 ans ou plus non diplômées ou dont le diplôme le plus élevé est inférieur à celui du baccalauréat (CAP ou BEP) sur l'ensemble des femmes non scolarisées de 15 ans ou plus.  Il s'agit d'un indicateur de frein potentiel à l'accès à l'emploi des femmes. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;53,9%&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+Pour les hommes comme pour les femmes, on observe un lien direct entre le niveau de diplôme et la probabilité d'être au chômage : plus le niveau de diplôme est bas, plus le risque de connaître des périodes de chômage est élevé. Or, si les femmes sont plus fréquemment diplômées du supérieur que les hommes, elles sont également plus souvent non diplômées que les hommes. En outre, les femmes ont plus tendances que les hommes à occuper des postes dont le niveau de qualification est inférieur à leur diplôme.&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Cet indicateur correspond à la part des enfants de moins de 3 ans qui n'ont théoriquement pas de place d'accueil (individuel ou collectif).  Il s'agit d'un indicateur de frein potentiel à l'accès à l'emploi des femmes.  En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;43,4 pour 100 enfants&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+Le fait d'avoir un ou plusieurs enfants dont au moins un en bas âge a un lien direct avec le taux d'emploi des femmes, en particulier dans le cas des familles nombreuses. A contrario, le taux d'emploi des hommes n'est que faiblement impacté par le nombre et l'âge de leurs enfants. Cet état de fait traduit les inégalités persistantes dans la répartition du travail domestique et en particulier du soin des enfants et souligne l'importance de la mise à disposition de places d'accueil en nombre suffisant dans le cadre de l'amélioration de l'accès à l'emploi des femmes.&lt;br/&gt;&lt;br/&gt;
+Pour aller plus loin : &lt;a href = 'http://www.caf.fr/sites/default/files/cnaf/Documents/Dser/observatoire_petite_enfance/Accueil-Jeune-Enfant_2017-donnees2016.pdf' target = '_blank'&gt;Observatoire National de la Petite Enfance (ONAPE), « L'accueil du jeune enfant en 2016. Données statistiques »&lt;/a&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'éloignement à l'école est mesuré par la proportion d'enfants de 6 à 10 ans qui fréquentent une école située en-dehors de leur commune de résidence. Il s'agit d'un indicateur de frein potentiel à l'accès à l'emploi des femmes.  En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;20,2%&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+Du fait de l'inégale répartition du travail domestique et en particulier du temps consacré au soin de enfants, les femmes sont souvent celles qui accompagnent les enfants à l'école. Les contraintes horaires qu'impliquent cette activité peuvent restreindre les possibilités d'emploi des femmes et justifier leur plus grand recours au temps partiel.&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;
+</t>
+  </si>
+  <si>
+    <t>Le temps moyen de trajet domicile-travail des femmes est modélisé à partir du distancier Metric de l'Insee à partir des communes de résidence et d'emploi des personnes enquêtées dans le cadre du recensement de la population. Ces distances sont une estimation par la route en période d'heures pleines.  Il s'agit d'un indicateur de frein potentiel à l'accès à l'emploi des femmes. En France (hors Mayotte), cet indicateur a une valeur de &lt;strong&gt;16 minutes&lt;/strong&gt;.&lt;br/&gt;&lt;br/&gt;
+Cet indicateur peut fortement varier selon les territoires. Les espaces situés à proximité des grandes agglomérations sont particulièrement concernés par des temps de trajet domicile-travail plus longs qu'ailleurs. La longueur des trajets domicile-travail peut constituer un frein pour l'accès à l'emploi des femmes dont l'emploi du temps est plus contraint que celui des hommes dans la mesure où c'est toujours à elles qu'échoit la majeure partie du travail domestique (accompagnement des enfants, achats, démarches,...). Les femmes ont ainsi plus tendance à résider près de leur travail que les hommes. &lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cette typologie a été réalisée à partir des 5 indicateurs d'accès à l'emploi des femmes (part d'inactives - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hors étudiantes et retraitées</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, taux de chômage des femmes, part d'emplois féminins à temps partiel, part d'emplois féminins précaires, part de jeunes femmes non insérées) et des 8 indicateurs de freins potentiels à l'emploi (part des familles monoparentales, part des familles nombreuses, part de emplois dans des CSP non mixtes, part des élèves de niveau 1ère inscrits dans des formations non-mixtes, part des femmes peu ou pas diplômées, part des enfants de moins de 3 ans n'ayant théoriquement pas de place d'accueil, part des enfants scolarisés hors de leur commune de résidence, temps moyen de trajet domicile-travail des femmes). Une mesure des inégalités femmes-hommes en termes d'accès à l'emploi compléte ce jeu de données. Il correspond à la somme des différences femmes-hommes en base 100 (en référence à la valeur nationale femmes) observées pour les indicateurs d'accès à l'emploi. &lt;br/&gt;&lt;br/&gt;
+Cette typologie est issue d'une classification ascendante hiérarchique opérée sur les 5 premiers axes de l'analyse en composantes principales résumant 72% de l'information contenue dans les 14 variables quantitatives utilisées pour l'analyse.&lt;br/&gt;&lt;br/&gt;
+&lt;i&gt;Attention : toute typologie résultant d'une simplification de la réalité, la description générale de chaque classe peut parfois entrer en contradiction avec certaines données détaillées présentées dans l'application sur certains points. &lt;/i&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;i class="fa fa-lightbulb"&gt;&lt;/i&gt;&lt;span style = 'color : #333232;font-style : italic ;'&gt;&amp;nbsp;&amp;nbsp;Cliquez sur la carte pour accéder à la cartothèque du CGET et télécharger la carte&lt;/span&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -446,7 +537,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,12 +580,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -508,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -538,12 +623,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1454,526 +1549,551 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="69.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3" style="17" customWidth="1"/>
+    <col min="2" max="2" width="7" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="17" customWidth="1"/>
+    <col min="8" max="9" width="69.140625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I9" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="I10" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="15" t="s">
+      <c r="H13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="15" t="s">
+      <c r="I13" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="C15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="H15" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="15" t="s">
+      <c r="I15" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="L15" s="20" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B2:J14">

</xml_diff>